<commit_message>
Fix missing policy ID number for Reduce BAU Subsidies [biomass] policy in WebAppData
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.2.3-indonesia-v3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-indonesia\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3534303-761F-4780-9CAD-98498A4EE077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="51195" windowHeight="18240"/>
+    <workbookView xWindow="2490" yWindow="1020" windowWidth="24765" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -22,8 +23,16 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PolicyLevers!$A$1:$Q$255</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -32,12 +41,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jeffrey Rissman</author>
   </authors>
   <commentList>
-    <comment ref="L2" authorId="0" shapeId="0">
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L86" authorId="0" shapeId="0">
+    <comment ref="L86" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -90,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2051" uniqueCount="811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="811">
   <si>
     <t>Short Name</t>
   </si>
@@ -2710,7 +2719,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -3593,6 +3602,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3602,23 +3614,20 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="Body: normal cell 2" xfId="5"/>
-    <cellStyle name="Comma 6" xfId="6"/>
+    <cellStyle name="Body: normal cell 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma 6" xfId="6" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Header: bottom row 2" xfId="4"/>
+    <cellStyle name="Header: bottom row 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3651,7 +3660,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3706,7 +3721,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3761,7 +3782,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3816,7 +3843,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4128,7 +4161,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -4199,7 +4232,7 @@
     <row r="17" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A10" r:id="rId1"/>
+    <hyperlink ref="A10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -4207,7 +4240,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U272"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4221,9 +4254,9 @@
     <col min="2" max="2" width="28.42578125" style="6" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" style="2" customWidth="1"/>
     <col min="4" max="5" width="18.85546875" style="6" customWidth="1"/>
-    <col min="6" max="7" width="18.42578125" style="6" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="21.28515625" style="8" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="21.28515625" style="6" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="18.42578125" style="6" customWidth="1"/>
+    <col min="8" max="9" width="21.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" style="6" customWidth="1"/>
     <col min="11" max="12" width="21.28515625" style="125" customWidth="1"/>
     <col min="13" max="13" width="19" style="6" customWidth="1"/>
     <col min="14" max="15" width="19.140625" style="2" customWidth="1"/>
@@ -13378,8 +13411,8 @@
         <v>116</v>
       </c>
       <c r="G180" s="6"/>
-      <c r="H180" s="8" t="s">
-        <v>237</v>
+      <c r="H180" s="8">
+        <v>185</v>
       </c>
       <c r="I180" s="12" t="str">
         <f t="shared" si="70"/>
@@ -18091,7 +18124,7 @@
       <c r="L272" s="136"/>
     </row>
   </sheetData>
-  <sortState ref="A119:I139">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A119:I139">
     <sortCondition ref="B119:B139"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18104,7 +18137,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18814,7 +18847,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -18856,7 +18889,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -18943,7 +18976,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AM194"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -18973,13 +19006,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
+      <c r="B1" s="148"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="152" t="s">
@@ -19048,13 +19081,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="151" t="s">
+      <c r="A60" s="148" t="s">
         <v>205</v>
       </c>
-      <c r="B60" s="151"/>
-      <c r="C60" s="151"/>
-      <c r="D60" s="151"/>
-      <c r="E60" s="151"/>
+      <c r="B60" s="148"/>
+      <c r="C60" s="148"/>
+      <c r="D60" s="148"/>
+      <c r="E60" s="148"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="65"/>
@@ -19166,13 +19199,13 @@
       </c>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A89" s="151" t="s">
+      <c r="A89" s="148" t="s">
         <v>206</v>
       </c>
-      <c r="B89" s="151"/>
-      <c r="C89" s="151"/>
-      <c r="D89" s="151"/>
-      <c r="E89" s="151"/>
+      <c r="B89" s="148"/>
+      <c r="C89" s="148"/>
+      <c r="D89" s="148"/>
+      <c r="E89" s="148"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
@@ -19259,13 +19292,13 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="151" t="s">
+      <c r="A98" s="148" t="s">
         <v>207</v>
       </c>
-      <c r="B98" s="151"/>
-      <c r="C98" s="151"/>
-      <c r="D98" s="151"/>
-      <c r="E98" s="151"/>
+      <c r="B98" s="148"/>
+      <c r="C98" s="148"/>
+      <c r="D98" s="148"/>
+      <c r="E98" s="148"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="42">
@@ -19349,13 +19382,13 @@
       <c r="A108" s="69"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="151" t="s">
+      <c r="A109" s="148" t="s">
         <v>209</v>
       </c>
-      <c r="B109" s="151"/>
-      <c r="C109" s="151"/>
-      <c r="D109" s="151"/>
-      <c r="E109" s="151"/>
+      <c r="B109" s="148"/>
+      <c r="C109" s="148"/>
+      <c r="D109" s="148"/>
+      <c r="E109" s="148"/>
     </row>
     <row r="110" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19368,13 +19401,13 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A113" s="151" t="s">
+      <c r="A113" s="148" t="s">
         <v>208</v>
       </c>
-      <c r="B113" s="151"/>
-      <c r="C113" s="151"/>
-      <c r="D113" s="151"/>
-      <c r="E113" s="151"/>
+      <c r="B113" s="148"/>
+      <c r="C113" s="148"/>
+      <c r="D113" s="148"/>
+      <c r="E113" s="148"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="42">
@@ -19455,13 +19488,13 @@
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A124" s="151" t="s">
+      <c r="A124" s="148" t="s">
         <v>499</v>
       </c>
-      <c r="B124" s="151"/>
-      <c r="C124" s="151"/>
-      <c r="D124" s="151"/>
-      <c r="E124" s="151"/>
+      <c r="B124" s="148"/>
+      <c r="C124" s="148"/>
+      <c r="D124" s="148"/>
+      <c r="E124" s="148"/>
       <c r="L124" s="44"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.25">
@@ -19552,13 +19585,13 @@
       <c r="C133" s="43"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A134" s="151" t="s">
+      <c r="A134" s="148" t="s">
         <v>125</v>
       </c>
-      <c r="B134" s="151"/>
-      <c r="C134" s="151"/>
-      <c r="D134" s="151"/>
-      <c r="E134" s="151"/>
+      <c r="B134" s="148"/>
+      <c r="C134" s="148"/>
+      <c r="D134" s="148"/>
+      <c r="E134" s="148"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="76" t="s">
@@ -19573,25 +19606,25 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="78"/>
-      <c r="B136" s="148" t="s">
+      <c r="B136" s="149" t="s">
         <v>521</v>
       </c>
-      <c r="C136" s="149"/>
-      <c r="D136" s="149"/>
-      <c r="E136" s="150"/>
+      <c r="C136" s="150"/>
+      <c r="D136" s="150"/>
+      <c r="E136" s="151"/>
       <c r="F136" s="77"/>
       <c r="G136" s="77"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="79"/>
-      <c r="B137" s="148" t="s">
+      <c r="B137" s="149" t="s">
         <v>522</v>
       </c>
-      <c r="C137" s="150"/>
-      <c r="D137" s="148" t="s">
+      <c r="C137" s="151"/>
+      <c r="D137" s="149" t="s">
         <v>523</v>
       </c>
-      <c r="E137" s="150"/>
+      <c r="E137" s="151"/>
       <c r="F137" s="77"/>
       <c r="G137" s="77"/>
     </row>
@@ -20138,13 +20171,13 @@
       <c r="G163" s="77"/>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A165" s="151" t="s">
+      <c r="A165" s="148" t="s">
         <v>212</v>
       </c>
-      <c r="B165" s="151"/>
-      <c r="C165" s="151"/>
-      <c r="D165" s="151"/>
-      <c r="E165" s="151"/>
+      <c r="B165" s="148"/>
+      <c r="C165" s="148"/>
+      <c r="D165" s="148"/>
+      <c r="E165" s="148"/>
       <c r="H165"/>
     </row>
     <row r="166" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20171,10 +20204,10 @@
       <c r="H168"/>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A169" s="151" t="s">
+      <c r="A169" s="148" t="s">
         <v>507</v>
       </c>
-      <c r="B169" s="151"/>
+      <c r="B169" s="148"/>
       <c r="H169"/>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
@@ -20209,13 +20242,13 @@
       <c r="B173" s="55"/>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A174" s="151" t="s">
+      <c r="A174" s="148" t="s">
         <v>222</v>
       </c>
-      <c r="B174" s="151"/>
-      <c r="C174" s="151"/>
-      <c r="D174" s="151"/>
-      <c r="E174" s="151"/>
+      <c r="B174" s="148"/>
+      <c r="C174" s="148"/>
+      <c r="D174" s="148"/>
+      <c r="E174" s="148"/>
     </row>
     <row r="175" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="46" t="s">
@@ -20235,13 +20268,13 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" s="151" t="s">
+      <c r="A178" s="148" t="s">
         <v>215</v>
       </c>
-      <c r="B178" s="151"/>
-      <c r="C178" s="151"/>
-      <c r="D178" s="151"/>
-      <c r="E178" s="151"/>
+      <c r="B178" s="148"/>
+      <c r="C178" s="148"/>
+      <c r="D178" s="148"/>
+      <c r="E178" s="148"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="47" t="s">
@@ -20269,13 +20302,13 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" s="151" t="s">
+      <c r="A183" s="148" t="s">
         <v>217</v>
       </c>
-      <c r="B183" s="151"/>
-      <c r="C183" s="151"/>
-      <c r="D183" s="151"/>
-      <c r="E183" s="151"/>
+      <c r="B183" s="148"/>
+      <c r="C183" s="148"/>
+      <c r="D183" s="148"/>
+      <c r="E183" s="148"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="74" t="s">
@@ -20309,13 +20342,13 @@
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" s="151" t="s">
+      <c r="A188" s="148" t="s">
         <v>234</v>
       </c>
-      <c r="B188" s="151"/>
-      <c r="C188" s="151"/>
-      <c r="D188" s="151"/>
-      <c r="E188" s="151"/>
+      <c r="B188" s="148"/>
+      <c r="C188" s="148"/>
+      <c r="D188" s="148"/>
+      <c r="E188" s="148"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="44" t="s">
@@ -20375,12 +20408,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A188:E188"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -20395,6 +20422,12 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
+    <mergeCell ref="A188:E188"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated webapp for new server
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-indonesia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Indonesia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3534303-761F-4780-9CAD-98498A4EE077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C46FAD-C8B9-4B84-A5E0-307B4238E940}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="1020" windowWidth="24765" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11280" yWindow="285" windowWidth="17310" windowHeight="16095" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
     <sheet name="PolicyLevers" sheetId="1" r:id="rId2"/>
     <sheet name="OutputGraphs" sheetId="8" r:id="rId3"/>
     <sheet name="ReferenceScenarios" sheetId="9" r:id="rId4"/>
-    <sheet name="Targets" sheetId="14" r:id="rId5"/>
+    <sheet name="Target Calculations" sheetId="14" r:id="rId5"/>
     <sheet name="MaxBoundCalculations" sheetId="13" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PolicyLevers!$A$1:$Q$255</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="824">
   <si>
     <t>Short Name</t>
   </si>
@@ -2714,6 +2714,45 @@
   </si>
   <si>
     <t>Output Total CO Emissions</t>
+  </si>
+  <si>
+    <t>Scenario_BAU.cin</t>
+  </si>
+  <si>
+    <t>Include?</t>
+  </si>
+  <si>
+    <t>Target 1 Title</t>
+  </si>
+  <si>
+    <t>Target 1 Year</t>
+  </si>
+  <si>
+    <t>Target 1 Min Value</t>
+  </si>
+  <si>
+    <t>Target 1 Max Value</t>
+  </si>
+  <si>
+    <t>Target 1 Description</t>
+  </si>
+  <si>
+    <t>Target 2 Title</t>
+  </si>
+  <si>
+    <t>Target 2 Year</t>
+  </si>
+  <si>
+    <t>Target 2 Min Value</t>
+  </si>
+  <si>
+    <t>Target 2 Max Value</t>
+  </si>
+  <si>
+    <t>Target 2 Description</t>
+  </si>
+  <si>
+    <t>reduction wedge</t>
   </si>
 </sst>
 </file>
@@ -3213,7 +3252,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3602,9 +3641,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3614,8 +3650,17 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -3630,7 +3675,28 @@
     <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4164,7 +4230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -18138,709 +18204,903 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.85546875" style="125" customWidth="1"/>
     <col min="2" max="2" width="37.5703125" style="125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="125" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="69" style="6" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="28" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="6"/>
+    <col min="3" max="3" width="15.7109375" style="125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="125" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="69" style="6" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="28" style="6" customWidth="1"/>
+    <col min="10" max="18" width="22" style="125" customWidth="1"/>
+    <col min="19" max="19" width="25.42578125" style="125" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="144" t="s">
         <v>756</v>
       </c>
       <c r="B1" s="145" t="s">
         <v>757</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="153" t="s">
+        <v>812</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="145" t="s">
+      <c r="H1" s="145" t="s">
         <v>763</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="270" x14ac:dyDescent="0.25">
       <c r="A2" s="146" t="s">
         <v>758</v>
       </c>
       <c r="B2" s="132" t="s">
         <v>759</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="154">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="125" t="s">
+      <c r="E2" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="J2" s="125" t="str">
+        <f>'Target Calculations'!A2</f>
+        <v>Unconditional Target</v>
+      </c>
+      <c r="K2" s="125">
+        <f>'Target Calculations'!B2</f>
+        <v>2030</v>
+      </c>
+      <c r="L2" s="125">
+        <f>'Target Calculations'!C2</f>
+        <v>2122.619728128268</v>
+      </c>
+      <c r="M2" s="125">
+        <f>'Target Calculations'!D2</f>
+        <v>2122.619728128268</v>
+      </c>
+      <c r="N2" s="125" t="str">
+        <f>'Target Calculations'!E2</f>
+        <v>In its Nationally Determined Contribution (NDC) to the U.N. Framework Convention on Climate Change, Indonesia committed to reduce greenhouse gas emissions 29 percent relative to a business-as-usual case by 2030.</v>
+      </c>
+      <c r="O2" s="125" t="str">
+        <f>'Target Calculations'!A3</f>
+        <v>Conditional Target</v>
+      </c>
+      <c r="P2" s="125">
+        <f>'Target Calculations'!B3</f>
+        <v>2030</v>
+      </c>
+      <c r="Q2" s="125">
+        <f>'Target Calculations'!C3</f>
+        <v>1864.8581387242943</v>
+      </c>
+      <c r="R2" s="125">
+        <f>'Target Calculations'!D3</f>
+        <v>1864.8581387242943</v>
+      </c>
+      <c r="S2" s="125" t="str">
+        <f>'Target Calculations'!E3</f>
+        <v>In its Nationally Determined Contribution (NDC) to the U.N. Framework Convention on Climate Change, Indonesia committed to reduce greenhouse gas emissions up to 41 percent relative to a business-as-usual case by 2030, subject to availability of international support for finance, technology transfer, and development and capacity-building.</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="146" t="s">
         <v>758</v>
       </c>
       <c r="B3" s="131" t="s">
         <v>760</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="154">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="125" t="s">
+      <c r="E3" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>746</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>619</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="131" t="s">
         <v>785</v>
       </c>
       <c r="B4" s="131" t="s">
         <v>786</v>
       </c>
-      <c r="C4" s="132" t="s">
+      <c r="C4" s="154">
+        <v>1</v>
+      </c>
+      <c r="D4" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="132" t="s">
+      <c r="E4" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="132" t="s">
+      <c r="F4" s="132" t="s">
         <v>464</v>
       </c>
-      <c r="F4" s="132" t="s">
+      <c r="G4" s="132" t="s">
         <v>787</v>
       </c>
-      <c r="G4" s="132"/>
-    </row>
-    <row r="5" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="132"/>
+    </row>
+    <row r="5" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="131" t="s">
         <v>785</v>
       </c>
       <c r="B5" s="146" t="s">
         <v>788</v>
       </c>
-      <c r="C5" s="132" t="s">
+      <c r="C5" s="154">
+        <v>1</v>
+      </c>
+      <c r="D5" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="132" t="s">
+      <c r="E5" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="132" t="s">
+      <c r="F5" s="132" t="s">
         <v>464</v>
       </c>
-      <c r="F5" s="132" t="s">
+      <c r="G5" s="132" t="s">
         <v>789</v>
       </c>
-      <c r="G5" s="132"/>
-    </row>
-    <row r="6" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="132"/>
+    </row>
+    <row r="6" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="131" t="s">
         <v>785</v>
       </c>
       <c r="B6" s="146" t="s">
         <v>790</v>
       </c>
-      <c r="C6" s="132" t="s">
+      <c r="C6" s="154">
+        <v>1</v>
+      </c>
+      <c r="D6" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="132" t="s">
+      <c r="E6" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="132" t="s">
+      <c r="F6" s="132" t="s">
         <v>464</v>
       </c>
-      <c r="F6" s="132" t="s">
+      <c r="G6" s="132" t="s">
         <v>791</v>
       </c>
-      <c r="G6" s="132"/>
-    </row>
-    <row r="7" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="132"/>
+    </row>
+    <row r="7" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="131" t="s">
         <v>785</v>
       </c>
       <c r="B7" s="146" t="s">
         <v>792</v>
       </c>
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="154">
+        <v>1</v>
+      </c>
+      <c r="D7" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="E7" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="132" t="s">
+      <c r="F7" s="132" t="s">
         <v>464</v>
       </c>
-      <c r="F7" s="132" t="s">
+      <c r="G7" s="132" t="s">
         <v>793</v>
       </c>
-      <c r="G7" s="132"/>
-    </row>
-    <row r="8" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="132"/>
+    </row>
+    <row r="8" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="131" t="s">
         <v>785</v>
       </c>
       <c r="B8" s="146" t="s">
         <v>794</v>
       </c>
-      <c r="C8" s="132" t="s">
+      <c r="C8" s="154">
+        <v>1</v>
+      </c>
+      <c r="D8" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="132" t="s">
+      <c r="E8" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="132" t="s">
+      <c r="F8" s="132" t="s">
         <v>795</v>
       </c>
-      <c r="F8" s="132" t="s">
+      <c r="G8" s="132" t="s">
         <v>796</v>
       </c>
-      <c r="G8" s="132"/>
-    </row>
-    <row r="9" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="132"/>
+    </row>
+    <row r="9" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="131" t="s">
         <v>785</v>
       </c>
       <c r="B9" s="146" t="s">
         <v>797</v>
       </c>
-      <c r="C9" s="132" t="s">
+      <c r="C9" s="154">
+        <v>1</v>
+      </c>
+      <c r="D9" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="132" t="s">
+      <c r="E9" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="132" t="s">
+      <c r="F9" s="132" t="s">
         <v>795</v>
       </c>
-      <c r="F9" s="132" t="s">
+      <c r="G9" s="132" t="s">
         <v>798</v>
       </c>
-      <c r="G9" s="132"/>
-    </row>
-    <row r="10" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="132"/>
+    </row>
+    <row r="10" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="131" t="s">
         <v>785</v>
       </c>
       <c r="B10" s="146" t="s">
         <v>799</v>
       </c>
-      <c r="C10" s="132" t="s">
+      <c r="C10" s="154">
+        <v>1</v>
+      </c>
+      <c r="D10" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="132" t="s">
+      <c r="E10" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="132" t="s">
+      <c r="F10" s="132" t="s">
         <v>795</v>
       </c>
-      <c r="F10" s="132" t="s">
+      <c r="G10" s="132" t="s">
         <v>800</v>
       </c>
-      <c r="G10" s="132"/>
-    </row>
-    <row r="11" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="132"/>
+    </row>
+    <row r="11" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="131" t="s">
         <v>785</v>
       </c>
       <c r="B11" s="146" t="s">
         <v>801</v>
       </c>
-      <c r="C11" s="132" t="s">
+      <c r="C11" s="154">
+        <v>1</v>
+      </c>
+      <c r="D11" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="132" t="s">
+      <c r="E11" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="132" t="s">
+      <c r="F11" s="132" t="s">
         <v>795</v>
       </c>
-      <c r="F11" s="132" t="s">
+      <c r="G11" s="132" t="s">
         <v>802</v>
       </c>
-      <c r="G11" s="132"/>
-    </row>
-    <row r="12" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="132"/>
+    </row>
+    <row r="12" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="131" t="s">
         <v>785</v>
       </c>
       <c r="B12" s="146" t="s">
         <v>803</v>
       </c>
-      <c r="C12" s="132" t="s">
+      <c r="C12" s="154">
+        <v>1</v>
+      </c>
+      <c r="D12" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="132" t="s">
+      <c r="E12" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="132" t="s">
+      <c r="F12" s="132" t="s">
         <v>464</v>
       </c>
-      <c r="F12" s="132" t="s">
+      <c r="G12" s="132" t="s">
         <v>804</v>
       </c>
-      <c r="G12" s="132"/>
-    </row>
-    <row r="13" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="132"/>
+    </row>
+    <row r="13" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="131" t="s">
         <v>785</v>
       </c>
       <c r="B13" s="146" t="s">
         <v>805</v>
       </c>
-      <c r="C13" s="132" t="s">
+      <c r="C13" s="154">
+        <v>1</v>
+      </c>
+      <c r="D13" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="132" t="s">
+      <c r="E13" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E13" s="132" t="s">
+      <c r="F13" s="132" t="s">
         <v>795</v>
       </c>
-      <c r="F13" s="132" t="s">
+      <c r="G13" s="132" t="s">
         <v>806</v>
       </c>
-      <c r="G13" s="132"/>
-    </row>
-    <row r="14" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="132"/>
+    </row>
+    <row r="14" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="131" t="s">
         <v>785</v>
       </c>
       <c r="B14" s="146" t="s">
         <v>807</v>
       </c>
-      <c r="C14" s="132" t="s">
+      <c r="C14" s="154">
+        <v>1</v>
+      </c>
+      <c r="D14" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="132" t="s">
+      <c r="E14" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="132" t="s">
+      <c r="F14" s="132" t="s">
         <v>464</v>
       </c>
-      <c r="F14" s="132" t="s">
+      <c r="G14" s="132" t="s">
         <v>808</v>
       </c>
-      <c r="G14" s="132"/>
-    </row>
-    <row r="15" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="132"/>
+    </row>
+    <row r="15" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="131" t="s">
         <v>785</v>
       </c>
       <c r="B15" s="146" t="s">
         <v>809</v>
       </c>
-      <c r="C15" s="132" t="s">
+      <c r="C15" s="154">
+        <v>1</v>
+      </c>
+      <c r="D15" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="132" t="s">
+      <c r="E15" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="132" t="s">
+      <c r="F15" s="132" t="s">
         <v>464</v>
       </c>
-      <c r="F15" s="132" t="s">
+      <c r="G15" s="132" t="s">
         <v>810</v>
       </c>
-      <c r="G15" s="132"/>
-    </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="132"/>
+    </row>
+    <row r="16" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="131" t="s">
         <v>468</v>
       </c>
       <c r="B16" s="120"/>
-      <c r="C16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="120" t="s">
+      <c r="C16" s="154">
+        <v>1</v>
+      </c>
+      <c r="D16" s="125" t="s">
+        <v>823</v>
+      </c>
+      <c r="E16" s="120" t="s">
         <v>730</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="G16" s="6" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="J16" s="120"/>
+      <c r="K16" s="120"/>
+      <c r="L16" s="120"/>
+      <c r="M16" s="120"/>
+      <c r="N16" s="120"/>
+      <c r="O16" s="120"/>
+      <c r="P16" s="120"/>
+      <c r="Q16" s="120"/>
+      <c r="R16" s="120"/>
+      <c r="S16" s="120"/>
+    </row>
+    <row r="17" spans="1:19" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="131" t="s">
         <v>469</v>
       </c>
       <c r="B17" s="131" t="s">
         <v>761</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="154">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="120" t="s">
+      <c r="E17" s="120" t="s">
         <v>731</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>747</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" s="120" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="J17" s="120"/>
+      <c r="K17" s="120"/>
+      <c r="L17" s="120"/>
+      <c r="M17" s="120"/>
+      <c r="N17" s="120"/>
+      <c r="O17" s="120"/>
+      <c r="P17" s="120"/>
+      <c r="Q17" s="120"/>
+      <c r="R17" s="120"/>
+      <c r="S17" s="120"/>
+    </row>
+    <row r="18" spans="1:19" s="120" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="131" t="s">
         <v>469</v>
       </c>
       <c r="B18" s="131" t="s">
         <v>762</v>
       </c>
-      <c r="C18" s="120" t="s">
+      <c r="C18" s="154">
+        <v>1</v>
+      </c>
+      <c r="D18" s="120" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="120" t="s">
+      <c r="E18" s="120" t="s">
         <v>731</v>
       </c>
-      <c r="E18" s="120" t="s">
+      <c r="F18" s="120" t="s">
         <v>735</v>
       </c>
-      <c r="F18" s="120" t="s">
+      <c r="G18" s="120" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="131" t="s">
         <v>764</v>
       </c>
       <c r="B19" s="131" t="s">
         <v>765</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="154">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="125" t="s">
+      <c r="E19" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>736</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>748</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="H19" s="6" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="131" t="s">
         <v>764</v>
       </c>
       <c r="B20" s="131" t="s">
         <v>766</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="154">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="125" t="s">
+      <c r="E20" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>736</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>749</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="H20" s="6" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="131" t="s">
         <v>764</v>
       </c>
       <c r="B21" s="131" t="s">
         <v>767</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="154">
+        <v>1</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="125" t="s">
+      <c r="E21" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>750</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="H21" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="131" t="s">
         <v>768</v>
       </c>
       <c r="B22" s="131" t="s">
         <v>769</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="154">
+        <v>1</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D22" s="125" t="s">
+      <c r="E22" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="131" t="s">
         <v>768</v>
       </c>
       <c r="B23" s="131" t="s">
         <v>770</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="154">
+        <v>1</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="125" t="s">
+      <c r="E23" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="131" t="s">
         <v>771</v>
       </c>
       <c r="B24" s="131" t="s">
         <v>772</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="154">
+        <v>1</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D24" s="125" t="s">
+      <c r="E24" s="125" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>751</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="H24" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="I24" s="6" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="131" t="s">
         <v>771</v>
       </c>
       <c r="B25" s="131" t="s">
         <v>773</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="154">
+        <v>1</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D25" s="125" t="s">
+      <c r="E25" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="H25" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="I25" s="6" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="135" x14ac:dyDescent="0.25">
       <c r="A26" s="131" t="s">
         <v>771</v>
       </c>
       <c r="B26" s="131" t="s">
         <v>774</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="154">
+        <v>1</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D26" s="125" t="s">
+      <c r="E26" s="125" t="s">
         <v>82</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="H26" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="I26" s="6" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A27" s="131" t="s">
         <v>771</v>
       </c>
       <c r="B27" s="131" t="s">
         <v>775</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="154">
+        <v>1</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D27" s="125" t="s">
+      <c r="E27" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>754</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="H27" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="I27" s="6" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="131" t="s">
         <v>738</v>
       </c>
       <c r="B28" s="131" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="132" t="s">
+      <c r="C28" s="154">
+        <v>1</v>
+      </c>
+      <c r="D28" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="132" t="s">
+      <c r="E28" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="132" t="s">
+      <c r="F28" s="132" t="s">
         <v>466</v>
       </c>
-      <c r="F28" s="132" t="s">
+      <c r="G28" s="132" t="s">
         <v>776</v>
       </c>
-      <c r="G28" s="132"/>
-    </row>
-    <row r="29" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="132"/>
+    </row>
+    <row r="29" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="131" t="s">
         <v>738</v>
       </c>
       <c r="B29" s="131" t="s">
         <v>777</v>
       </c>
-      <c r="C29" s="132" t="s">
+      <c r="C29" s="154">
+        <v>1</v>
+      </c>
+      <c r="D29" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D29" s="132" t="s">
+      <c r="E29" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E29" s="125" t="s">
+      <c r="F29" s="125" t="s">
         <v>778</v>
       </c>
-      <c r="F29" s="132" t="s">
+      <c r="G29" s="132" t="s">
         <v>784</v>
       </c>
-      <c r="G29" s="132"/>
-    </row>
-    <row r="30" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="132"/>
+    </row>
+    <row r="30" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="131" t="s">
         <v>738</v>
       </c>
       <c r="B30" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="132" t="s">
+      <c r="C30" s="154">
+        <v>1</v>
+      </c>
+      <c r="D30" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="132" t="s">
+      <c r="E30" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E30" s="125" t="s">
+      <c r="F30" s="125" t="s">
         <v>779</v>
       </c>
-      <c r="F30" s="132" t="s">
+      <c r="G30" s="132" t="s">
         <v>780</v>
       </c>
-      <c r="G30" s="132"/>
-    </row>
-    <row r="31" spans="1:8" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="132"/>
+    </row>
+    <row r="31" spans="1:19" s="147" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="131" t="s">
         <v>738</v>
       </c>
       <c r="B31" s="131" t="s">
         <v>781</v>
       </c>
-      <c r="C31" s="132" t="s">
+      <c r="C31" s="154">
+        <v>1</v>
+      </c>
+      <c r="D31" s="132" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="132" t="s">
+      <c r="E31" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="125" t="s">
+      <c r="F31" s="125" t="s">
         <v>782</v>
       </c>
-      <c r="F31" s="132" t="s">
+      <c r="G31" s="132" t="s">
         <v>783</v>
       </c>
-      <c r="G31" s="132"/>
+      <c r="H31" s="132"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C31">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -18850,7 +19110,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18871,7 +19133,7 @@
         <v>183</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>811</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -18892,7 +19154,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19006,13 +19270,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="151" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="148"/>
-      <c r="C1" s="148"/>
-      <c r="D1" s="148"/>
-      <c r="E1" s="148"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="152" t="s">
@@ -19081,13 +19345,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="148" t="s">
+      <c r="A60" s="151" t="s">
         <v>205</v>
       </c>
-      <c r="B60" s="148"/>
-      <c r="C60" s="148"/>
-      <c r="D60" s="148"/>
-      <c r="E60" s="148"/>
+      <c r="B60" s="151"/>
+      <c r="C60" s="151"/>
+      <c r="D60" s="151"/>
+      <c r="E60" s="151"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="65"/>
@@ -19199,13 +19463,13 @@
       </c>
     </row>
     <row r="89" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A89" s="148" t="s">
+      <c r="A89" s="151" t="s">
         <v>206</v>
       </c>
-      <c r="B89" s="148"/>
-      <c r="C89" s="148"/>
-      <c r="D89" s="148"/>
-      <c r="E89" s="148"/>
+      <c r="B89" s="151"/>
+      <c r="C89" s="151"/>
+      <c r="D89" s="151"/>
+      <c r="E89" s="151"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
@@ -19292,13 +19556,13 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="148" t="s">
+      <c r="A98" s="151" t="s">
         <v>207</v>
       </c>
-      <c r="B98" s="148"/>
-      <c r="C98" s="148"/>
-      <c r="D98" s="148"/>
-      <c r="E98" s="148"/>
+      <c r="B98" s="151"/>
+      <c r="C98" s="151"/>
+      <c r="D98" s="151"/>
+      <c r="E98" s="151"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="42">
@@ -19382,13 +19646,13 @@
       <c r="A108" s="69"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="148" t="s">
+      <c r="A109" s="151" t="s">
         <v>209</v>
       </c>
-      <c r="B109" s="148"/>
-      <c r="C109" s="148"/>
-      <c r="D109" s="148"/>
-      <c r="E109" s="148"/>
+      <c r="B109" s="151"/>
+      <c r="C109" s="151"/>
+      <c r="D109" s="151"/>
+      <c r="E109" s="151"/>
     </row>
     <row r="110" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19401,13 +19665,13 @@
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A113" s="148" t="s">
+      <c r="A113" s="151" t="s">
         <v>208</v>
       </c>
-      <c r="B113" s="148"/>
-      <c r="C113" s="148"/>
-      <c r="D113" s="148"/>
-      <c r="E113" s="148"/>
+      <c r="B113" s="151"/>
+      <c r="C113" s="151"/>
+      <c r="D113" s="151"/>
+      <c r="E113" s="151"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="42">
@@ -19488,13 +19752,13 @@
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A124" s="148" t="s">
+      <c r="A124" s="151" t="s">
         <v>499</v>
       </c>
-      <c r="B124" s="148"/>
-      <c r="C124" s="148"/>
-      <c r="D124" s="148"/>
-      <c r="E124" s="148"/>
+      <c r="B124" s="151"/>
+      <c r="C124" s="151"/>
+      <c r="D124" s="151"/>
+      <c r="E124" s="151"/>
       <c r="L124" s="44"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.25">
@@ -19585,13 +19849,13 @@
       <c r="C133" s="43"/>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A134" s="148" t="s">
+      <c r="A134" s="151" t="s">
         <v>125</v>
       </c>
-      <c r="B134" s="148"/>
-      <c r="C134" s="148"/>
-      <c r="D134" s="148"/>
-      <c r="E134" s="148"/>
+      <c r="B134" s="151"/>
+      <c r="C134" s="151"/>
+      <c r="D134" s="151"/>
+      <c r="E134" s="151"/>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="76" t="s">
@@ -19606,25 +19870,25 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="78"/>
-      <c r="B136" s="149" t="s">
+      <c r="B136" s="148" t="s">
         <v>521</v>
       </c>
-      <c r="C136" s="150"/>
-      <c r="D136" s="150"/>
-      <c r="E136" s="151"/>
+      <c r="C136" s="149"/>
+      <c r="D136" s="149"/>
+      <c r="E136" s="150"/>
       <c r="F136" s="77"/>
       <c r="G136" s="77"/>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="79"/>
-      <c r="B137" s="149" t="s">
+      <c r="B137" s="148" t="s">
         <v>522</v>
       </c>
-      <c r="C137" s="151"/>
-      <c r="D137" s="149" t="s">
+      <c r="C137" s="150"/>
+      <c r="D137" s="148" t="s">
         <v>523</v>
       </c>
-      <c r="E137" s="151"/>
+      <c r="E137" s="150"/>
       <c r="F137" s="77"/>
       <c r="G137" s="77"/>
     </row>
@@ -20171,13 +20435,13 @@
       <c r="G163" s="77"/>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A165" s="148" t="s">
+      <c r="A165" s="151" t="s">
         <v>212</v>
       </c>
-      <c r="B165" s="148"/>
-      <c r="C165" s="148"/>
-      <c r="D165" s="148"/>
-      <c r="E165" s="148"/>
+      <c r="B165" s="151"/>
+      <c r="C165" s="151"/>
+      <c r="D165" s="151"/>
+      <c r="E165" s="151"/>
       <c r="H165"/>
     </row>
     <row r="166" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20204,10 +20468,10 @@
       <c r="H168"/>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A169" s="148" t="s">
+      <c r="A169" s="151" t="s">
         <v>507</v>
       </c>
-      <c r="B169" s="148"/>
+      <c r="B169" s="151"/>
       <c r="H169"/>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
@@ -20242,13 +20506,13 @@
       <c r="B173" s="55"/>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A174" s="148" t="s">
+      <c r="A174" s="151" t="s">
         <v>222</v>
       </c>
-      <c r="B174" s="148"/>
-      <c r="C174" s="148"/>
-      <c r="D174" s="148"/>
-      <c r="E174" s="148"/>
+      <c r="B174" s="151"/>
+      <c r="C174" s="151"/>
+      <c r="D174" s="151"/>
+      <c r="E174" s="151"/>
     </row>
     <row r="175" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="46" t="s">
@@ -20268,13 +20532,13 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" s="148" t="s">
+      <c r="A178" s="151" t="s">
         <v>215</v>
       </c>
-      <c r="B178" s="148"/>
-      <c r="C178" s="148"/>
-      <c r="D178" s="148"/>
-      <c r="E178" s="148"/>
+      <c r="B178" s="151"/>
+      <c r="C178" s="151"/>
+      <c r="D178" s="151"/>
+      <c r="E178" s="151"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="47" t="s">
@@ -20302,13 +20566,13 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" s="148" t="s">
+      <c r="A183" s="151" t="s">
         <v>217</v>
       </c>
-      <c r="B183" s="148"/>
-      <c r="C183" s="148"/>
-      <c r="D183" s="148"/>
-      <c r="E183" s="148"/>
+      <c r="B183" s="151"/>
+      <c r="C183" s="151"/>
+      <c r="D183" s="151"/>
+      <c r="E183" s="151"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="74" t="s">
@@ -20342,13 +20606,13 @@
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" s="148" t="s">
+      <c r="A188" s="151" t="s">
         <v>234</v>
       </c>
-      <c r="B188" s="148"/>
-      <c r="C188" s="148"/>
-      <c r="D188" s="148"/>
-      <c r="E188" s="148"/>
+      <c r="B188" s="151"/>
+      <c r="C188" s="151"/>
+      <c r="D188" s="151"/>
+      <c r="E188" s="151"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="44" t="s">
@@ -20408,6 +20672,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A188:E188"/>
+    <mergeCell ref="A165:E165"/>
+    <mergeCell ref="A178:E178"/>
+    <mergeCell ref="A183:E183"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A169:B169"/>
     <mergeCell ref="B136:E136"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="D137:E137"/>
@@ -20422,12 +20692,6 @@
     <mergeCell ref="A113:E113"/>
     <mergeCell ref="A109:E109"/>
     <mergeCell ref="A124:E124"/>
-    <mergeCell ref="A188:E188"/>
-    <mergeCell ref="A165:E165"/>
-    <mergeCell ref="A178:E178"/>
-    <mergeCell ref="A183:E183"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A169:B169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>